<commit_message>
feat: Complete invoice automation system with OCR, AI extraction, and cloud storage
- Added OpenRouter AI integration for intelligent data extraction
- Implemented multiple cloud storage options (Telegram, MEGA, Google Drive)
- Added document embedding feature (Aadhaar, DL) in Excel invoices
- Created comprehensive documentation and deployment guides
- Added invoice counter management with financial year tracking
- Improved Excel template handling with formula preservation
- Enhanced web UI with multiple file upload support
- Added fallback extraction for better reliability
</commit_message>
<xml_diff>
--- a/inn sample.xlsx
+++ b/inn sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\users\asus\Desktop\Invoice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20989C3C-56E1-4169-A9FC-79BC42A7703E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181141D6-DC55-4728-90A7-2D617B2A21BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{E5274884-9083-419E-935C-37BBD2D76392}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>TAX INVOICE</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>INVOICE NO.</t>
-  </si>
-  <si>
-    <t>HD/2025-26/034</t>
   </si>
   <si>
     <t>INVOICE DATE</t>
@@ -709,77 +706,77 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,8 +1117,8 @@
   </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="75" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1157,7 +1154,7 @@
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="44" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="37"/>
@@ -1168,7 +1165,7 @@
     <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="45" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="37"/>
@@ -1179,7 +1176,7 @@
     <row r="5" spans="1:9" ht="15.75" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="45" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="37"/>
@@ -1190,7 +1187,7 @@
     <row r="6" spans="1:9" ht="15.75" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="46" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="37"/>
@@ -1209,22 +1206,20 @@
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1235,9 +1230,9 @@
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="56"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="47"/>
       <c r="C10" s="37"/>
       <c r="D10" s="37"/>
       <c r="E10" s="5"/>
@@ -1246,20 +1241,20 @@
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B11" s="62"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="37"/>
       <c r="D11" s="37"/>
       <c r="E11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="38" t="s">
         <v>12</v>
-      </c>
-      <c r="F11" s="63" t="s">
-        <v>13</v>
       </c>
       <c r="G11" s="39"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="37"/>
       <c r="C12" s="37"/>
@@ -1280,23 +1275,23 @@
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="F14" s="47"/>
       <c r="G14" s="39"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="47" t="s">
         <v>17</v>
-      </c>
-      <c r="B15" s="56" t="s">
-        <v>18</v>
       </c>
       <c r="C15" s="37"/>
       <c r="D15" s="37"/>
@@ -1315,25 +1310,25 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="C17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="D17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="F17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="G17" s="15" t="s">
         <v>24</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.5">
@@ -1377,7 +1372,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="11">
         <v>150</v>
@@ -1390,7 +1385,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="23"/>
@@ -1416,181 +1411,181 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="D25" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="D25" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="45"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="51"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="57">
+      <c r="E26" s="49"/>
+      <c r="F26" s="50">
         <v>0</v>
       </c>
-      <c r="G26" s="45"/>
+      <c r="G26" s="51"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="D27" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="50">
+      <c r="E27" s="49"/>
+      <c r="F27" s="53">
         <f>E18</f>
         <v>0</v>
       </c>
-      <c r="G27" s="45"/>
+      <c r="G27" s="51"/>
     </row>
     <row r="28" spans="1:7" ht="13.9">
       <c r="A28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="D28" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="53" t="s">
+      <c r="E28" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="50">
+      <c r="F28" s="53">
         <f>E18*0.025</f>
         <v>0</v>
       </c>
-      <c r="G28" s="45"/>
+      <c r="G28" s="51"/>
     </row>
     <row r="29" spans="1:7" ht="13.9">
       <c r="A29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="D29" s="55"/>
+      <c r="E29" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="54"/>
-      <c r="E29" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="50">
+      <c r="F29" s="53">
         <f>E18*0.025</f>
         <v>0</v>
       </c>
-      <c r="G29" s="45"/>
+      <c r="G29" s="51"/>
     </row>
     <row r="30" spans="1:7" ht="13.9">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
-      <c r="D30" s="55"/>
+      <c r="D30" s="56"/>
       <c r="E30" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="50"/>
-      <c r="G30" s="45"/>
+        <v>41</v>
+      </c>
+      <c r="F30" s="53"/>
+      <c r="G30" s="51"/>
     </row>
     <row r="31" spans="1:7" ht="13.9">
       <c r="A31" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="D31" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="45"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="51"/>
     </row>
     <row r="32" spans="1:7" ht="13.9">
       <c r="A32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="D32" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="D32" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="43"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="45"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="51"/>
     </row>
     <row r="33" spans="1:7" ht="27.75">
       <c r="A33" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="64"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="43"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="45"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="51"/>
     </row>
     <row r="34" spans="1:7" ht="13.9">
       <c r="A34" s="29"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="42" t="s">
+      <c r="B34" s="42"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="49"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="51"/>
+    </row>
+    <row r="35" spans="1:7" ht="13.9">
+      <c r="A35" s="61" t="s">
         <v>50</v>
-      </c>
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="45"/>
-    </row>
-    <row r="35" spans="1:7" ht="13.9">
-      <c r="A35" s="46" t="s">
-        <v>51</v>
       </c>
       <c r="B35" s="37"/>
       <c r="C35" s="37"/>
-      <c r="D35" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="44">
+      <c r="D35" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="49"/>
+      <c r="F35" s="60">
         <f>F33:G33-F34:G34</f>
         <v>0</v>
       </c>
-      <c r="G35" s="45"/>
+      <c r="G35" s="51"/>
     </row>
     <row r="36" spans="1:7" ht="12.75">
-      <c r="A36" s="41"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="37"/>
       <c r="C36" s="37"/>
       <c r="G36" s="30"/>
     </row>
     <row r="37" spans="1:7" ht="13.9">
-      <c r="A37" s="41"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="37"/>
       <c r="C37" s="37"/>
-      <c r="D37" s="48" t="s">
-        <v>53</v>
+      <c r="D37" s="63" t="s">
+        <v>52</v>
       </c>
       <c r="E37" s="37"/>
-      <c r="F37" s="49"/>
+      <c r="F37" s="64"/>
       <c r="G37" s="39"/>
     </row>
     <row r="38" spans="1:7" ht="13.9">
       <c r="A38" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -1598,32 +1593,32 @@
       <c r="G38" s="39"/>
     </row>
     <row r="39" spans="1:7" ht="13.5">
-      <c r="A39" s="36" t="s">
-        <v>55</v>
+      <c r="A39" s="65" t="s">
+        <v>54</v>
       </c>
       <c r="B39" s="37"/>
       <c r="C39" s="37"/>
       <c r="G39" s="30"/>
     </row>
     <row r="40" spans="1:7" ht="13.5">
-      <c r="A40" s="36" t="s">
-        <v>56</v>
+      <c r="A40" s="65" t="s">
+        <v>55</v>
       </c>
       <c r="B40" s="37"/>
       <c r="C40" s="37"/>
       <c r="G40" s="30"/>
     </row>
     <row r="41" spans="1:7" ht="13.5">
-      <c r="A41" s="36" t="s">
-        <v>57</v>
+      <c r="A41" s="65" t="s">
+        <v>56</v>
       </c>
       <c r="B41" s="37"/>
       <c r="C41" s="37"/>
       <c r="G41" s="30"/>
     </row>
     <row r="42" spans="1:7" ht="13.5">
-      <c r="A42" s="36" t="s">
-        <v>58</v>
+      <c r="A42" s="65" t="s">
+        <v>57</v>
       </c>
       <c r="B42" s="37"/>
       <c r="C42" s="37"/>
@@ -1631,22 +1626,22 @@
       <c r="G42" s="30"/>
     </row>
     <row r="43" spans="1:7" ht="12.75">
-      <c r="A43" s="40" t="s">
-        <v>59</v>
+      <c r="A43" s="67" t="s">
+        <v>58</v>
       </c>
       <c r="B43" s="37"/>
       <c r="C43" s="37"/>
       <c r="G43" s="30"/>
     </row>
     <row r="44" spans="1:7" ht="12.75">
-      <c r="A44" s="41"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="37"/>
       <c r="C44" s="37"/>
       <c r="G44" s="30"/>
     </row>
     <row r="45" spans="1:7" ht="13.5">
-      <c r="A45" s="36" t="s">
-        <v>60</v>
+      <c r="A45" s="65" t="s">
+        <v>59</v>
       </c>
       <c r="B45" s="37"/>
       <c r="C45" s="37"/>
@@ -1654,13 +1649,13 @@
       <c r="G45" s="30"/>
     </row>
     <row r="46" spans="1:7" ht="13.5">
-      <c r="A46" s="36" t="s">
-        <v>61</v>
+      <c r="A46" s="65" t="s">
+        <v>60</v>
       </c>
       <c r="B46" s="37"/>
       <c r="C46" s="37"/>
-      <c r="E46" s="38" t="s">
-        <v>62</v>
+      <c r="E46" s="66" t="s">
+        <v>61</v>
       </c>
       <c r="F46" s="37"/>
       <c r="G46" s="39"/>
@@ -1685,6 +1680,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="E46:G47"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:C44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A35:C37"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G38"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
     <mergeCell ref="B11:D13"/>
     <mergeCell ref="F11:G13"/>
     <mergeCell ref="B33:C34"/>
@@ -1701,31 +1721,6 @@
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="F27:G27"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:C37"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G38"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="E46:G47"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:C44"/>
-    <mergeCell ref="A45:D45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{472A8773-D07F-4008-9689-F6FC1BF92061}"/>

</xml_diff>